<commit_message>
migrating to Python 3
</commit_message>
<xml_diff>
--- a/examples/demo/data/scenarios.xlsx
+++ b/examples/demo/data/scenarios.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84887840-5A4C-4912-A298-40653F249075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SolverSettings" sheetId="2" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="54">
   <si>
     <t>Scenario</t>
   </si>
@@ -181,12 +182,15 @@
   </si>
   <si>
     <t>MinGrowthSeed</t>
+  </si>
+  <si>
+    <t>MaxLoan_yrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,19 +502,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -544,7 +548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -561,7 +565,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -578,7 +582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -595,7 +599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -612,7 +616,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -629,7 +633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -644,6 +648,23 @@
       </c>
       <c r="E8">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -653,19 +674,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -699,7 +720,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -716,7 +737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -733,7 +754,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -750,7 +771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -767,7 +788,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -784,7 +805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -801,7 +822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -818,7 +839,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -835,7 +856,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -852,7 +873,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -869,7 +890,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -880,7 +901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -891,22 +912,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -917,7 +938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -928,7 +949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -939,7 +960,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -950,7 +971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -961,7 +982,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -972,7 +993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -983,7 +1004,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -994,7 +1015,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1005,7 +1026,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1016,7 +1037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1033,19 +1054,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1076,7 +1097,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1093,7 +1114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1110,7 +1131,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1127,7 +1148,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1144,7 +1165,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1161,7 +1182,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1178,7 +1199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -1195,7 +1216,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1218,19 +1239,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1264,7 +1285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -1281,7 +1302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>